<commit_message>
SM: add iteration 3 documents and update readme
</commit_message>
<xml_diff>
--- a/doc/CS673_SPPP_RiskManagement_team5.xlsx
+++ b/doc/CS673_SPPP_RiskManagement_team5.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="126">
   <si>
     <t>This sheet provides some common risks in student projects. You should check if it applies to your group project. 
 You should also feel free to add other risks. Exemplary analysis is also added.</t>
@@ -134,10 +134,7 @@
     <t>As long as we track our user stories and work. There shouldn't be anyone working on something someone already has. Each week we'll having meetings to communicate what each person is currently working on. So even if it does happen we will find out early</t>
   </si>
   <si>
-    <t>Communcating and assigning our names to things</t>
-  </si>
-  <si>
-    <t>Open</t>
+    <t>Everyone assigned a unique task to prevent repetition of the same work</t>
   </si>
   <si>
     <t>worked on wrong components</t>
@@ -152,6 +149,9 @@
     <t>As long as we track our user stories and work. There shouldn't be any discrepancy of anyone working on something that is unneeded</t>
   </si>
   <si>
+    <t>Everyone's responsibilites were laid out during weekly meetings</t>
+  </si>
+  <si>
     <t xml:space="preserve">Requirements </t>
   </si>
   <si>
@@ -167,7 +167,7 @@
     <t>Peer Review for requirements to make sure they are not ambiguous</t>
   </si>
   <si>
-    <t>As of week 1, requirements look good</t>
+    <t>Requirements were reviewed with team and clarified</t>
   </si>
   <si>
     <t>scope creep</t>
@@ -179,6 +179,9 @@
     <t>Devil's advocate for uncontrolled changes as one of the peer roles during review</t>
   </si>
   <si>
+    <t>Made sure to understand what we can't accomplish in time</t>
+  </si>
+  <si>
     <t>constant requirements changes</t>
   </si>
   <si>
@@ -188,6 +191,9 @@
     <t>Agile development will be required to know whether implementation is possible for each requirement, which means frequent review and implementation rather than having all requirements finalized before starting implementation</t>
   </si>
   <si>
+    <t>Requirements have been established and code has been completed for each</t>
+  </si>
+  <si>
     <t>Management</t>
   </si>
   <si>
@@ -203,7 +209,7 @@
     <t>Using JIRA we can accurately plan and keep track of the work.</t>
   </si>
   <si>
-    <t>So far we are planning everything together and making decisions as a group so everyone is on the same page</t>
+    <t>Planned everything together and makde decisions as a group so everyone was on the same page</t>
   </si>
   <si>
     <t>lack of management skills</t>
@@ -218,7 +224,7 @@
     <t>Management is very important, to keep team members motivated and on the correct track. With out management there is no accountability to make sure something gets done. Weekly meetings and JIRA planning will help with the management aspects</t>
   </si>
   <si>
-    <t>We are having weekly meetings, with agendas to make sure everyone knows what to have done by a certain time period</t>
+    <t>We had weekly meetings, with agendas to make sure everyone knows what to have done by a certain time period. veryone was able to complete their parts.</t>
   </si>
   <si>
     <t>Technology competence</t>
@@ -238,7 +244,7 @@
 Implement a basic application using Flask</t>
   </si>
   <si>
-    <t>Lazaro willing to teach</t>
+    <t>Everyone as able to learn Flask enough to complete their respective functionality by getting help from others and online resources</t>
   </si>
   <si>
     <t>Not familiar with the programming language used</t>
@@ -346,6 +352,9 @@
     <t>Code Review for Pull Requests to make sure all codes are understandable</t>
   </si>
   <si>
+    <t>Code has been completed and reviewed using PRs</t>
+  </si>
+  <si>
     <t xml:space="preserve">Testing </t>
   </si>
   <si>
@@ -361,7 +370,7 @@
     <t>Devlopment and testing will be done simultanesouly</t>
   </si>
   <si>
-    <t>Development has not started yet</t>
+    <t>Unit tests, automated tests, and functional tests were completed</t>
   </si>
   <si>
     <t>Improper testing tools</t>
@@ -373,6 +382,9 @@
     <t xml:space="preserve">Gathering the proper tools for testing our code </t>
   </si>
   <si>
+    <t>Selenium used for automated tests</t>
+  </si>
+  <si>
     <t>Integration and deployment</t>
   </si>
   <si>
@@ -385,6 +397,9 @@
     <t>Start researching ways in which we would need to integrate the tools we are using for the project</t>
   </si>
   <si>
+    <t>Deployment giving trouble, but continued work is being done. Deployment was complete</t>
+  </si>
+  <si>
     <t>Integrations arent connecting</t>
   </si>
   <si>
@@ -392,6 +407,9 @@
   </si>
   <si>
     <t>List out contingencies where we would need to keep systems disperate</t>
+  </si>
+  <si>
+    <t>Tools were integrated</t>
   </si>
 </sst>
 </file>
@@ -1044,8 +1062,8 @@
       <c r="K6" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="L6" s="7" t="s">
-        <v>37</v>
+      <c r="L6" s="12" t="s">
+        <v>20</v>
       </c>
       <c r="M6" s="13"/>
       <c r="N6" s="13"/>
@@ -1066,10 +1084,10 @@
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="6"/>
       <c r="B7" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>38</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>39</v>
       </c>
       <c r="D7" s="15">
         <v>3.0</v>
@@ -1085,19 +1103,19 @@
         <v>36</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I7" s="16">
         <v>45217.0</v>
       </c>
       <c r="J7" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K7" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="K7" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="L7" s="7" t="s">
-        <v>37</v>
+      <c r="L7" s="12" t="s">
+        <v>20</v>
       </c>
       <c r="M7" s="13"/>
       <c r="N7" s="13"/>
@@ -1150,8 +1168,8 @@
       <c r="K8" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="L8" s="7" t="s">
-        <v>37</v>
+      <c r="L8" s="12" t="s">
+        <v>20</v>
       </c>
       <c r="M8" s="13"/>
       <c r="N8" s="13"/>
@@ -1200,10 +1218,10 @@
         <v>50</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="L9" s="7" t="s">
-        <v>37</v>
+        <v>51</v>
+      </c>
+      <c r="L9" s="12" t="s">
+        <v>20</v>
       </c>
       <c r="M9" s="13"/>
       <c r="N9" s="13"/>
@@ -1224,10 +1242,10 @@
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="14"/>
       <c r="B10" s="6" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D10" s="15">
         <v>3.0</v>
@@ -1249,13 +1267,13 @@
         <v>45195.0</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="L10" s="7" t="s">
-        <v>37</v>
+        <v>55</v>
+      </c>
+      <c r="L10" s="12" t="s">
+        <v>20</v>
       </c>
       <c r="M10" s="13"/>
       <c r="N10" s="13"/>
@@ -1275,13 +1293,13 @@
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="14" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D11" s="15">
         <v>1.0</v>
@@ -1297,19 +1315,19 @@
         <v>60</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="I11" s="16">
         <v>45217.0</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="L11" s="7" t="s">
-        <v>37</v>
+        <v>61</v>
+      </c>
+      <c r="L11" s="12" t="s">
+        <v>20</v>
       </c>
       <c r="M11" s="13"/>
       <c r="N11" s="13"/>
@@ -1330,10 +1348,10 @@
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="14"/>
       <c r="B12" s="18" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D12" s="15">
         <v>2.0</v>
@@ -1349,19 +1367,19 @@
         <v>48</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I12" s="16">
         <v>45217.0</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="K12" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="L12" s="7" t="s">
-        <v>37</v>
+        <v>66</v>
+      </c>
+      <c r="L12" s="12" t="s">
+        <v>20</v>
       </c>
       <c r="M12" s="13"/>
       <c r="N12" s="13"/>
@@ -1381,13 +1399,13 @@
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="14" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D13" s="15">
         <v>5.0</v>
@@ -1403,19 +1421,19 @@
         <v>9</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="I13" s="16">
         <v>45195.0</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="K13" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="L13" s="7" t="s">
-        <v>37</v>
+        <v>72</v>
+      </c>
+      <c r="L13" s="12" t="s">
+        <v>20</v>
       </c>
       <c r="M13" s="19"/>
       <c r="N13" s="13"/>
@@ -1436,10 +1454,10 @@
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="14"/>
       <c r="B14" s="6" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D14" s="15">
         <v>5.0</v>
@@ -1461,10 +1479,10 @@
         <v>45188.0</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="K14" s="5" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L14" s="12" t="s">
         <v>20</v>
@@ -1488,10 +1506,10 @@
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="14"/>
       <c r="B15" s="6" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D15" s="15">
         <v>4.0</v>
@@ -1513,10 +1531,10 @@
         <v>45202.0</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="K15" s="5" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="L15" s="12" t="s">
         <v>20</v>
@@ -1540,10 +1558,10 @@
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="14"/>
       <c r="B16" s="6" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D16" s="15">
         <v>5.0</v>
@@ -1559,16 +1577,16 @@
         <v>9</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="I16" s="16">
         <v>45195.0</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="L16" s="12" t="s">
         <v>20</v>
@@ -1592,10 +1610,10 @@
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="14"/>
       <c r="B17" s="6" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D17" s="15">
         <v>4.0</v>
@@ -1617,10 +1635,10 @@
         <v>45188.0</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="K17" s="5" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="L17" s="12" t="s">
         <v>20</v>
@@ -1644,10 +1662,10 @@
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="14"/>
       <c r="B18" s="17" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D18" s="15">
         <v>2.0</v>
@@ -1669,10 +1687,10 @@
         <v>45188.0</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="K18" s="5" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="L18" s="12" t="s">
         <v>20</v>
@@ -1695,13 +1713,13 @@
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="14" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D19" s="15">
         <v>3.0</v>
@@ -1717,16 +1735,16 @@
         <v>24</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="I19" s="16">
         <v>45195.0</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="K19" s="5" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="L19" s="12" t="s">
         <v>20</v>
@@ -1750,10 +1768,10 @@
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="14"/>
       <c r="B20" s="6" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D20" s="15">
         <v>2.0</v>
@@ -1769,16 +1787,16 @@
         <v>32</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="I20" s="16">
         <v>45195.0</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="K20" s="5" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="L20" s="12" t="s">
         <v>20</v>
@@ -1802,10 +1820,10 @@
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="14"/>
       <c r="B21" s="6" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D21" s="15">
         <v>4.0</v>
@@ -1821,19 +1839,19 @@
         <v>16</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="I21" s="16">
         <v>45217.0</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="K21" s="5" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="L21" s="12" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="M21" s="13"/>
       <c r="N21" s="13"/>
@@ -1853,13 +1871,13 @@
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="14" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="D22" s="15">
         <v>2.0</v>
@@ -1874,19 +1892,19 @@
         <v>4.0</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="I22" s="16">
         <v>45195.0</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="K22" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="L22" s="7" t="s">
-        <v>37</v>
+        <v>112</v>
+      </c>
+      <c r="L22" s="12" t="s">
+        <v>20</v>
       </c>
       <c r="M22" s="19"/>
       <c r="N22" s="13"/>
@@ -1907,10 +1925,10 @@
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="14"/>
       <c r="B23" s="17" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="D23" s="15">
         <v>2.0</v>
@@ -1925,16 +1943,16 @@
         <v>3.0</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="I23" s="16">
         <v>45195.0</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="K23" s="5" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="L23" s="12" t="s">
         <v>20</v>
@@ -1957,13 +1975,13 @@
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="14" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="B24" s="20" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="D24" s="15">
         <v>2.0</v>
@@ -1978,19 +1996,19 @@
         <v>3.0</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="I24" s="16">
         <v>45195.0</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="K24" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="L24" s="7" t="s">
-        <v>37</v>
+        <v>121</v>
+      </c>
+      <c r="L24" s="12" t="s">
+        <v>20</v>
       </c>
       <c r="M24" s="19"/>
       <c r="N24" s="13"/>
@@ -2011,10 +2029,10 @@
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="6"/>
       <c r="B25" s="17" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="D25" s="15">
         <v>2.0</v>
@@ -2029,16 +2047,16 @@
         <v>4.0</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="I25" s="16">
         <v>45195.0</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="K25" s="5" t="s">
-        <v>109</v>
+        <v>125</v>
       </c>
       <c r="L25" s="12" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
SM: removing heroku and adding in old documents
</commit_message>
<xml_diff>
--- a/doc/CS673_SPPP_RiskManagement_team5.xlsx
+++ b/doc/CS673_SPPP_RiskManagement_team5.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="126">
   <si>
     <t>This sheet provides some common risks in student projects. You should check if it applies to your group project. 
 You should also feel free to add other risks. Exemplary analysis is also added.</t>
@@ -134,10 +134,7 @@
     <t>As long as we track our user stories and work. There shouldn't be anyone working on something someone already has. Each week we'll having meetings to communicate what each person is currently working on. So even if it does happen we will find out early</t>
   </si>
   <si>
-    <t>Communcating and assigning our names to things</t>
-  </si>
-  <si>
-    <t>Open</t>
+    <t>Everyone assigned a unique task to prevent repetition of the same work</t>
   </si>
   <si>
     <t>worked on wrong components</t>
@@ -152,6 +149,9 @@
     <t>As long as we track our user stories and work. There shouldn't be any discrepancy of anyone working on something that is unneeded</t>
   </si>
   <si>
+    <t>Everyone's responsibilites were laid out during weekly meetings</t>
+  </si>
+  <si>
     <t xml:space="preserve">Requirements </t>
   </si>
   <si>
@@ -167,7 +167,7 @@
     <t>Peer Review for requirements to make sure they are not ambiguous</t>
   </si>
   <si>
-    <t>As of week 1, requirements look good</t>
+    <t>Requirements were reviewed with team and clarified</t>
   </si>
   <si>
     <t>scope creep</t>
@@ -179,6 +179,9 @@
     <t>Devil's advocate for uncontrolled changes as one of the peer roles during review</t>
   </si>
   <si>
+    <t>Made sure to understand what we can't accomplish in time</t>
+  </si>
+  <si>
     <t>constant requirements changes</t>
   </si>
   <si>
@@ -188,6 +191,9 @@
     <t>Agile development will be required to know whether implementation is possible for each requirement, which means frequent review and implementation rather than having all requirements finalized before starting implementation</t>
   </si>
   <si>
+    <t>Requirements have been established and code has been completed for each</t>
+  </si>
+  <si>
     <t>Management</t>
   </si>
   <si>
@@ -203,7 +209,7 @@
     <t>Using JIRA we can accurately plan and keep track of the work.</t>
   </si>
   <si>
-    <t>So far we are planning everything together and making decisions as a group so everyone is on the same page</t>
+    <t>Planned everything together and makde decisions as a group so everyone was on the same page</t>
   </si>
   <si>
     <t>lack of management skills</t>
@@ -218,7 +224,7 @@
     <t>Management is very important, to keep team members motivated and on the correct track. With out management there is no accountability to make sure something gets done. Weekly meetings and JIRA planning will help with the management aspects</t>
   </si>
   <si>
-    <t>We are having weekly meetings, with agendas to make sure everyone knows what to have done by a certain time period</t>
+    <t>We had weekly meetings, with agendas to make sure everyone knows what to have done by a certain time period. veryone was able to complete their parts.</t>
   </si>
   <si>
     <t>Technology competence</t>
@@ -238,7 +244,7 @@
 Implement a basic application using Flask</t>
   </si>
   <si>
-    <t>Lazaro willing to teach</t>
+    <t>Everyone as able to learn Flask enough to complete their respective functionality by getting help from others and online resources</t>
   </si>
   <si>
     <t>Not familiar with the programming language used</t>
@@ -346,6 +352,9 @@
     <t>Code Review for Pull Requests to make sure all codes are understandable</t>
   </si>
   <si>
+    <t>Code has been completed and reviewed using PRs</t>
+  </si>
+  <si>
     <t xml:space="preserve">Testing </t>
   </si>
   <si>
@@ -361,7 +370,7 @@
     <t>Devlopment and testing will be done simultanesouly</t>
   </si>
   <si>
-    <t>Development has not started yet</t>
+    <t>Unit tests, automated tests, and functional tests were completed</t>
   </si>
   <si>
     <t>Improper testing tools</t>
@@ -373,6 +382,9 @@
     <t xml:space="preserve">Gathering the proper tools for testing our code </t>
   </si>
   <si>
+    <t>Selenium used for automated tests</t>
+  </si>
+  <si>
     <t>Integration and deployment</t>
   </si>
   <si>
@@ -385,6 +397,9 @@
     <t>Start researching ways in which we would need to integrate the tools we are using for the project</t>
   </si>
   <si>
+    <t>Deployment giving trouble, but continued work is being done. Deployment was complete</t>
+  </si>
+  <si>
     <t>Integrations arent connecting</t>
   </si>
   <si>
@@ -392,6 +407,9 @@
   </si>
   <si>
     <t>List out contingencies where we would need to keep systems disperate</t>
+  </si>
+  <si>
+    <t>Tools were integrated</t>
   </si>
 </sst>
 </file>
@@ -1044,8 +1062,8 @@
       <c r="K6" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="L6" s="7" t="s">
-        <v>37</v>
+      <c r="L6" s="12" t="s">
+        <v>20</v>
       </c>
       <c r="M6" s="13"/>
       <c r="N6" s="13"/>
@@ -1066,10 +1084,10 @@
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="6"/>
       <c r="B7" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>38</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>39</v>
       </c>
       <c r="D7" s="15">
         <v>3.0</v>
@@ -1085,19 +1103,19 @@
         <v>36</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I7" s="16">
         <v>45217.0</v>
       </c>
       <c r="J7" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K7" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="K7" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="L7" s="7" t="s">
-        <v>37</v>
+      <c r="L7" s="12" t="s">
+        <v>20</v>
       </c>
       <c r="M7" s="13"/>
       <c r="N7" s="13"/>
@@ -1150,8 +1168,8 @@
       <c r="K8" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="L8" s="7" t="s">
-        <v>37</v>
+      <c r="L8" s="12" t="s">
+        <v>20</v>
       </c>
       <c r="M8" s="13"/>
       <c r="N8" s="13"/>
@@ -1200,10 +1218,10 @@
         <v>50</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="L9" s="7" t="s">
-        <v>37</v>
+        <v>51</v>
+      </c>
+      <c r="L9" s="12" t="s">
+        <v>20</v>
       </c>
       <c r="M9" s="13"/>
       <c r="N9" s="13"/>
@@ -1224,10 +1242,10 @@
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="14"/>
       <c r="B10" s="6" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D10" s="15">
         <v>3.0</v>
@@ -1249,13 +1267,13 @@
         <v>45195.0</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="L10" s="7" t="s">
-        <v>37</v>
+        <v>55</v>
+      </c>
+      <c r="L10" s="12" t="s">
+        <v>20</v>
       </c>
       <c r="M10" s="13"/>
       <c r="N10" s="13"/>
@@ -1275,13 +1293,13 @@
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="14" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D11" s="15">
         <v>1.0</v>
@@ -1297,19 +1315,19 @@
         <v>60</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="I11" s="16">
         <v>45217.0</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="L11" s="7" t="s">
-        <v>37</v>
+        <v>61</v>
+      </c>
+      <c r="L11" s="12" t="s">
+        <v>20</v>
       </c>
       <c r="M11" s="13"/>
       <c r="N11" s="13"/>
@@ -1330,10 +1348,10 @@
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="14"/>
       <c r="B12" s="18" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D12" s="15">
         <v>2.0</v>
@@ -1349,19 +1367,19 @@
         <v>48</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I12" s="16">
         <v>45217.0</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="K12" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="L12" s="7" t="s">
-        <v>37</v>
+        <v>66</v>
+      </c>
+      <c r="L12" s="12" t="s">
+        <v>20</v>
       </c>
       <c r="M12" s="13"/>
       <c r="N12" s="13"/>
@@ -1381,13 +1399,13 @@
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="14" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D13" s="15">
         <v>5.0</v>
@@ -1403,19 +1421,19 @@
         <v>9</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="I13" s="16">
         <v>45195.0</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="K13" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="L13" s="7" t="s">
-        <v>37</v>
+        <v>72</v>
+      </c>
+      <c r="L13" s="12" t="s">
+        <v>20</v>
       </c>
       <c r="M13" s="19"/>
       <c r="N13" s="13"/>
@@ -1436,10 +1454,10 @@
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="14"/>
       <c r="B14" s="6" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D14" s="15">
         <v>5.0</v>
@@ -1461,10 +1479,10 @@
         <v>45188.0</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="K14" s="5" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L14" s="12" t="s">
         <v>20</v>
@@ -1488,10 +1506,10 @@
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="14"/>
       <c r="B15" s="6" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D15" s="15">
         <v>4.0</v>
@@ -1513,10 +1531,10 @@
         <v>45202.0</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="K15" s="5" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="L15" s="12" t="s">
         <v>20</v>
@@ -1540,10 +1558,10 @@
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="14"/>
       <c r="B16" s="6" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D16" s="15">
         <v>5.0</v>
@@ -1559,16 +1577,16 @@
         <v>9</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="I16" s="16">
         <v>45195.0</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="L16" s="12" t="s">
         <v>20</v>
@@ -1592,10 +1610,10 @@
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="14"/>
       <c r="B17" s="6" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D17" s="15">
         <v>4.0</v>
@@ -1617,10 +1635,10 @@
         <v>45188.0</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="K17" s="5" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="L17" s="12" t="s">
         <v>20</v>
@@ -1644,10 +1662,10 @@
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="14"/>
       <c r="B18" s="17" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D18" s="15">
         <v>2.0</v>
@@ -1669,10 +1687,10 @@
         <v>45188.0</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="K18" s="5" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="L18" s="12" t="s">
         <v>20</v>
@@ -1695,13 +1713,13 @@
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="14" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D19" s="15">
         <v>3.0</v>
@@ -1717,16 +1735,16 @@
         <v>24</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="I19" s="16">
         <v>45195.0</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="K19" s="5" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="L19" s="12" t="s">
         <v>20</v>
@@ -1750,10 +1768,10 @@
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="14"/>
       <c r="B20" s="6" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D20" s="15">
         <v>2.0</v>
@@ -1769,16 +1787,16 @@
         <v>32</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="I20" s="16">
         <v>45195.0</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="K20" s="5" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="L20" s="12" t="s">
         <v>20</v>
@@ -1802,10 +1820,10 @@
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="14"/>
       <c r="B21" s="6" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D21" s="15">
         <v>4.0</v>
@@ -1821,19 +1839,19 @@
         <v>16</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="I21" s="16">
         <v>45217.0</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="K21" s="5" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="L21" s="12" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="M21" s="13"/>
       <c r="N21" s="13"/>
@@ -1853,13 +1871,13 @@
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="14" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="D22" s="15">
         <v>2.0</v>
@@ -1874,19 +1892,19 @@
         <v>4.0</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="I22" s="16">
         <v>45195.0</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="K22" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="L22" s="7" t="s">
-        <v>37</v>
+        <v>112</v>
+      </c>
+      <c r="L22" s="12" t="s">
+        <v>20</v>
       </c>
       <c r="M22" s="19"/>
       <c r="N22" s="13"/>
@@ -1907,10 +1925,10 @@
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="14"/>
       <c r="B23" s="17" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="D23" s="15">
         <v>2.0</v>
@@ -1925,16 +1943,16 @@
         <v>3.0</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="I23" s="16">
         <v>45195.0</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="K23" s="5" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="L23" s="12" t="s">
         <v>20</v>
@@ -1957,13 +1975,13 @@
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="14" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="B24" s="20" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="D24" s="15">
         <v>2.0</v>
@@ -1978,19 +1996,19 @@
         <v>3.0</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="I24" s="16">
         <v>45195.0</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="K24" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="L24" s="7" t="s">
-        <v>37</v>
+        <v>121</v>
+      </c>
+      <c r="L24" s="12" t="s">
+        <v>20</v>
       </c>
       <c r="M24" s="19"/>
       <c r="N24" s="13"/>
@@ -2011,10 +2029,10 @@
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="6"/>
       <c r="B25" s="17" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="D25" s="15">
         <v>2.0</v>
@@ -2029,16 +2047,16 @@
         <v>4.0</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="I25" s="16">
         <v>45195.0</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="K25" s="5" t="s">
-        <v>109</v>
+        <v>125</v>
       </c>
       <c r="L25" s="12" t="s">
         <v>20</v>

</xml_diff>